<commit_message>
Put the driver initialization and test data initialization in TestBase class
</commit_message>
<xml_diff>
--- a/target/classes/TestData/testdata.xlsx
+++ b/target/classes/TestData/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7485" tabRatio="755"/>
+    <workbookView windowWidth="19890" windowHeight="7425" tabRatio="755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Parameters</t>
   </si>
@@ -89,7 +89,7 @@
     <t>run</t>
   </si>
   <si>
-    <t>Ajay_yadav_4,Test@123</t>
+    <t>ajay_yadav_3,Test@123</t>
   </si>
 </sst>
 </file>
@@ -97,10 +97,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -124,6 +124,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -132,31 +139,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -170,82 +169,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,8 +220,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,6 +242,37 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -283,13 +283,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,25 +409,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,43 +439,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,91 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,12 +477,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -506,38 +519,28 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,20 +560,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,148 +579,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1129,8 +1129,8 @@
   <sheetPr/>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1241,7 +1241,7 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
completed JIRA integration with the framework
</commit_message>
<xml_diff>
--- a/target/classes/TestData/testdata.xlsx
+++ b/target/classes/TestData/testdata.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VibhorAgarwal/TGAF_Mobile/src/main/resources/TestData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="755"/>
+    <workbookView windowWidth="20490" windowHeight="7695" tabRatio="755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
     <sheet name="DemoTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Parameters</t>
   </si>
@@ -36,6 +26,9 @@
     <t>platform</t>
   </si>
   <si>
+    <t>android</t>
+  </si>
+  <si>
     <t>apkFileName</t>
   </si>
   <si>
@@ -66,15 +59,24 @@
     <t>deviceNameIOS</t>
   </si>
   <si>
+    <t>330061d0507945ff</t>
+  </si>
+  <si>
     <t>platformVersionIOS</t>
   </si>
   <si>
     <t>ipaFileName</t>
   </si>
   <si>
+    <t>app-stage-release-31-12-18.ipa</t>
+  </si>
+  <si>
     <t>udid</t>
   </si>
   <si>
+    <t>86916042-2875-47F2-9F72-D06D7C664BEA</t>
+  </si>
+  <si>
     <t>Test Case Name</t>
   </si>
   <si>
@@ -87,68 +89,32 @@
     <t>loginTest</t>
   </si>
   <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>ajay_yadav_3,Test@123</t>
+  </si>
+  <si>
+    <t>loginTest1</t>
+  </si>
+  <si>
     <t>run</t>
   </si>
   <si>
-    <t>ajay_yadav_3,Test@123</t>
-  </si>
-  <si>
-    <t>loginTest1</t>
-  </si>
-  <si>
     <t>ajay_yadav_3,Test@1234</t>
-  </si>
-  <si>
-    <t>HDFC_Investor.app</t>
-  </si>
-  <si>
-    <t>ff3d41c333c6ced1fe82eaaf15f826a27526c34c</t>
-  </si>
-  <si>
-    <t>xcodeOrgId</t>
-  </si>
-  <si>
-    <t>7993H7QQDX</t>
-  </si>
-  <si>
-    <t>xcodeSigningId</t>
-  </si>
-  <si>
-    <t>iPhone Developer</t>
-  </si>
-  <si>
-    <t>updateWDABundleId</t>
-  </si>
-  <si>
-    <t>com.ttndevelopment.hdfc</t>
-  </si>
-  <si>
-    <t>connectHardwareKeyboard</t>
-  </si>
-  <si>
-    <t>iPhone</t>
-  </si>
-  <si>
-    <t>IOS_XCUI_TEST</t>
-  </si>
-  <si>
-    <t>automationname</t>
-  </si>
-  <si>
-    <t>platformNameIOS</t>
-  </si>
-  <si>
-    <t>ios</t>
-  </si>
-  <si>
-    <t>iOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -168,16 +134,353 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -185,13 +488,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -204,14 +749,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -544,27 +1133,27 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" customWidth="1"/>
-    <col min="3" max="3" width="49.1640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="68.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="49.1619047619048" customWidth="1"/>
+    <col min="4" max="4" width="36.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" ht="23.25" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -572,191 +1161,144 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" ht="23.25" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="3" ht="23.25" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="4" ht="23.25" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="5" ht="23.25" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" ht="23.25" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" ht="23.25" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>4723</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" ht="23.25" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" ht="23.25" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" ht="23.25" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" ht="23.25" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="6">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="65.1640625" customWidth="1"/>
+    <col min="1" max="1" width="65.1619047619048" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.33203125" customWidth="1"/>
+    <col min="3" max="3" width="70.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" ht="23.25" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" ht="23.25" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" ht="23.25" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>